<commit_message>
reverted to text field
</commit_message>
<xml_diff>
--- a/extras/Sample form Conjoint Analysis.xlsx
+++ b/extras/Sample form Conjoint Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mitoworks/Downloads/GitHub/conjoint-analysis/extras/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6AD0C1-E920-FD4A-8E4D-F227A6720B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E956A0-B5F9-7747-B78B-92470CBD730C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34560" yWindow="-1540" windowWidth="25600" windowHeight="19980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34560" yWindow="-1540" windowWidth="25600" windowHeight="19980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="432">
   <si>
     <t>type</t>
   </si>
@@ -3065,12 +3065,6 @@
 &lt;br&gt;
 We will show you how to create multiple scenarios using a Repeat Group</t>
   </si>
-  <si>
-    <t>select_one placeholder</t>
-  </si>
-  <si>
-    <t>placeholder</t>
-  </si>
 </sst>
 </file>
 
@@ -5237,9 +5231,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1009"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6256,7 +6250,7 @@
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="22" t="s">
-        <v>432</v>
+        <v>59</v>
       </c>
       <c r="B30" s="23" t="s">
         <v>84</v>
@@ -34108,11 +34102,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Y1000"/>
+  <dimension ref="A1:Y999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -34255,15 +34249,9 @@
       <c r="Y4" s="4"/>
     </row>
     <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="59" t="s">
-        <v>433</v>
-      </c>
-      <c r="B5" s="59">
-        <v>1</v>
-      </c>
-      <c r="C5" s="59" t="s">
-        <v>433</v>
-      </c>
+      <c r="A5" s="59"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="59"/>
       <c r="E5" s="59"/>
       <c r="F5" s="4"/>
@@ -40065,33 +40053,7 @@
       <c r="X219" s="4"/>
       <c r="Y219" s="4"/>
     </row>
-    <row r="220" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A220" s="59"/>
-      <c r="B220" s="59"/>
-      <c r="C220" s="59"/>
-      <c r="D220" s="59"/>
-      <c r="E220" s="59"/>
-      <c r="F220" s="4"/>
-      <c r="G220" s="4"/>
-      <c r="H220" s="4"/>
-      <c r="I220" s="4"/>
-      <c r="J220" s="4"/>
-      <c r="K220" s="4"/>
-      <c r="L220" s="4"/>
-      <c r="M220" s="4"/>
-      <c r="N220" s="4"/>
-      <c r="O220" s="4"/>
-      <c r="P220" s="4"/>
-      <c r="Q220" s="4"/>
-      <c r="R220" s="4"/>
-      <c r="S220" s="4"/>
-      <c r="T220" s="4"/>
-      <c r="U220" s="4"/>
-      <c r="V220" s="4"/>
-      <c r="W220" s="4"/>
-      <c r="X220" s="4"/>
-      <c r="Y220" s="4"/>
-    </row>
+    <row r="220" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="221" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="222" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="223" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -40871,7 +40833,6 @@
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -40946,7 +40907,7 @@
       </c>
       <c r="C2" s="59" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2305261722</v>
+        <v>2306011500</v>
       </c>
       <c r="D2" s="62" t="s">
         <v>122</v>

</xml_diff>